<commit_message>
Cleanup: remove trailing spaces.
Command used: `for f in $(git ls-files); do sed -i 's/[ \t]*$//' "$f"; done`
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/template_mesh_generator.xlsx
+++ b/app/skinGui/iniGenerators/template_mesh_generator.xlsx
@@ -1,19 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="13455" yWindow="-15" windowWidth="11685" windowHeight="12120"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="145621"/>
-</workbook>
-</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
@@ -768,1318 +752,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>581602</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>108376</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>247971</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>157937</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="29" name="Group 28"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="11675426" y="2091817"/>
-          <a:ext cx="7566516" cy="5013767"/>
-          <a:chOff x="10981462" y="1799664"/>
-          <a:chExt cx="5588677" cy="4621561"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="28" name="Group 27"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="10981462" y="1799664"/>
-            <a:ext cx="5588677" cy="4621561"/>
-            <a:chOff x="10824580" y="1351429"/>
-            <a:chExt cx="5588677" cy="4621561"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="2" name="Picture 1" descr="Octagon.bmp"/>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10824580" y="1351429"/>
-              <a:ext cx="5588677" cy="4621561"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="27" name="Group 26"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="11384219" y="1533525"/>
-              <a:ext cx="4573401" cy="4017410"/>
-              <a:chOff x="11384219" y="1533525"/>
-              <a:chExt cx="4573401" cy="4017410"/>
-            </a:xfrm>
-          </xdr:grpSpPr>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="3" name="TextBox 2"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="12557313" y="5286375"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>1</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="4" name="TextBox 3"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="13192126" y="4849346"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>2</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="5" name="TextBox 4"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="14213543" y="5132854"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>3</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="6" name="TextBox 5"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="13805648" y="4248150"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>4</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="7" name="TextBox 6"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="13899778" y="3717552"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>5</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="9" name="TextBox 8"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="13829181" y="2614893"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="ctr"/>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>7</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="10" name="TextBox 9"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="13219580" y="2124075"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>8</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="11" name="TextBox 10"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="14144066" y="1905000"/>
-                <a:ext cx="283614" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>9</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="12" name="TextBox 11"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="12397251" y="2143125"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>11</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="13" name="TextBox 12"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="12597276" y="1533525"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>10</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="14" name="TextBox 13"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="12797301" y="2800350"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>12</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="15" name="TextBox 14"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="12049308" y="2486025"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>13</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="16" name="TextBox 15"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="12578226" y="3600450"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>14</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="17" name="TextBox 16"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="12154083" y="3933825"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>15</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="18" name="TextBox 17"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="11954058" y="4676775"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>16</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="19" name="TextBox 18"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="14751046" y="5010150"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>17</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="20" name="TextBox 19"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="14834530" y="3989294"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>18</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="21" name="TextBox 20"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="15320305" y="3727076"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>19</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="22" name="TextBox 21"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="15594850" y="2875429"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>20</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="23" name="TextBox 22"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="14979646" y="2533650"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>21</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="24" name="TextBox 23"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="11482291" y="2790825"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>22</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="25" name="TextBox 24"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="11384219" y="4268258"/>
-                <a:ext cx="362770" cy="264560"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="3">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>23</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="TextBox 7"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="14379949" y="3376893"/>
-            <a:ext cx="283614" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="3">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="3">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>6</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T55"/>
@@ -3576,28 +2248,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>